<commit_message>
Add HSI Review Sheet Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/HSI/HSI_Review.xlsx
+++ b/Input documents/HSI/HSI_Review.xlsx
@@ -157,7 +157,7 @@
   </si>
   <si>
     <t xml:space="preserve">In section 3.3.5 ATMEGA32 :
-There is no need to add this kind of information as it is outside the scope of HSI document. </t>
+There is no need to add this kind of information as it is outside the scope of HSI document.</t>
   </si>
   <si>
     <t xml:space="preserve">Resolved</t>
@@ -186,7 +186,7 @@
     <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
     <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -231,12 +231,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -421,7 +415,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -514,22 +508,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -550,7 +532,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -558,7 +540,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -714,7 +696,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
   </cols>
@@ -956,10 +938,10 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
@@ -1026,13 +1008,13 @@
       <c r="I2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -1041,7 +1023,7 @@
       <c r="E3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="23" t="s">
         <v>34</v>
       </c>
       <c r="G3" s="22"/>
@@ -1054,22 +1036,22 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="18" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>37</v>
       </c>
       <c r="G4" s="22"/>
@@ -1079,13 +1061,13 @@
       <c r="I4" s="22"/>
     </row>
     <row r="5" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="18" t="s">
@@ -1094,7 +1076,7 @@
       <c r="E5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="23" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="22"/>
@@ -1104,13 +1086,13 @@
       <c r="I5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -1132,13 +1114,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -1249,356 +1231,356 @@
       <c r="I14" s="20"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
-      <c r="I15" s="32"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
-      <c r="I16" s="32"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="31"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
-      <c r="I17" s="32"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
-      <c r="I18" s="32"/>
+      <c r="I18" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="34"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
-      <c r="I19" s="32"/>
+      <c r="I19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="18"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="32"/>
+      <c r="I20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="18"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="22"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="32"/>
+      <c r="I22" s="29"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="32"/>
+      <c r="I23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
-      <c r="I24" s="32"/>
+      <c r="I24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
-      <c r="I25" s="32"/>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
-      <c r="I26" s="32"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="34"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="31"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
-      <c r="I27" s="32"/>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="34"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
-      <c r="I28" s="32"/>
+      <c r="I28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
-      <c r="I29" s="32"/>
+      <c r="I29" s="29"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="35"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="32"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
-      <c r="I30" s="32"/>
+      <c r="I30" s="29"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="34"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="31"/>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
-      <c r="I31" s="32"/>
+      <c r="I31" s="29"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="34"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
-      <c r="I32" s="32"/>
+      <c r="I32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="34"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
-      <c r="I33" s="32"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="34"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
-      <c r="I34" s="32"/>
+      <c r="I34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="34"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
-      <c r="I35" s="32"/>
+      <c r="I35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="34"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
-      <c r="I36" s="32"/>
+      <c r="I36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="34"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
-      <c r="I37" s="32"/>
+      <c r="I37" s="29"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="34"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="32"/>
+      <c r="I38" s="29"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="34"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="31"/>
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="32"/>
+      <c r="I39" s="29"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="34"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="31"/>
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
-      <c r="I40" s="32"/>
+      <c r="I40" s="29"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="34"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="31"/>
       <c r="G41" s="22"/>
       <c r="H41" s="22"/>
-      <c r="I41" s="32"/>
+      <c r="I41" s="29"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="34"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="31"/>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
-      <c r="I42" s="32"/>
+      <c r="I42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="34"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="31"/>
       <c r="G43" s="22"/>
       <c r="H43" s="22"/>
-      <c r="I43" s="32"/>
+      <c r="I43" s="29"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="34"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="31"/>
       <c r="G44" s="22"/>
       <c r="H44" s="22"/>
-      <c r="I44" s="32"/>
+      <c r="I44" s="29"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="34"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="31"/>
       <c r="G45" s="22"/>
       <c r="H45" s="22"/>
-      <c r="I45" s="32"/>
+      <c r="I45" s="29"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="34"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="31"/>
       <c r="G46" s="22"/>
       <c r="H46" s="22"/>
-      <c r="I46" s="32"/>
+      <c r="I46" s="29"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1608,7 +1590,7 @@
       <formula>#ref!</formula>
     </cfRule>
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>#REF!</formula>
+      <formula>#ref!</formula>
     </cfRule>
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>#ref!</formula>

</xml_diff>